<commit_message>
hore: mise à jour effectuée
</commit_message>
<xml_diff>
--- a/data/LAHINIRIKO JULIEN TSILAGNOSY.xlsx
+++ b/data/LAHINIRIKO JULIEN TSILAGNOSY.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,15 +471,20 @@
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
+          <t>Fotoana</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
           <t>gender</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>dob</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>religion</t>
         </is>
@@ -496,12 +501,14 @@
           <t xml:space="preserve">TJN </t>
         </is>
       </c>
-      <c r="C2" t="n">
-        <v>346117893</v>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>0346117893</t>
+        </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>RAZAFINDRATSARA JUSTIN BOB</t>
+          <t>RABEMILSON FRED</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
@@ -512,116 +519,27 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Mpandrafitra</t>
+          <t>Miasa</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
+          <t xml:space="preserve">Jeudi </t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
           <t>homme</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="J2" t="inlineStr">
         <is>
           <t>12/03/2005</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Luthérien </t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">LAHINIRIKO JULIEN TSILAGNOSY </t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">TJN </t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>346117893</v>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">PASCAL John Gabriel </t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Mahavoky </t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>Mpandrafitra</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>homme</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>25/06/1999</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Temoin de Jéhovah </t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">LAHINIRIKO JULIEN TSILAGNOSY </t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">TJN </t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>0346117893</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">PASCAL John Gabriel </t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Mahavoky </t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>Mpandrafitra</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>homme</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>25/06/1999</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Temoin de Jéhovah </t>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>hindouisme</t>
         </is>
       </c>
     </row>

</xml_diff>